<commit_message>
Retested previous bugs on Version 2 of the website
</commit_message>
<xml_diff>
--- a/test-cases.xlsx
+++ b/test-cases.xlsx
@@ -8,28 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Desktop\testing-stuff\banking-application-testing-Guru99\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F80037C-BC4F-44C3-86AE-591FBB33D246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D0FC09-CA56-49D9-8013-EE79D29F7130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="New Customer" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
-    <sheet name="Changelog" sheetId="2" r:id="rId3"/>
-    <sheet name="FundTransfer" sheetId="3" state="hidden" r:id="rId4"/>
-    <sheet name="BalenceEnquiry" sheetId="4" state="hidden" r:id="rId5"/>
-    <sheet name="Inter Bank Fund  Transfer" sheetId="5" state="hidden" r:id="rId6"/>
-    <sheet name="Change  password" sheetId="6" state="hidden" r:id="rId7"/>
+    <sheet name="Unit Testing" sheetId="1" r:id="rId1"/>
+    <sheet name="Integration Testing" sheetId="8" r:id="rId2"/>
+    <sheet name="Demo Credentials" sheetId="7" r:id="rId3"/>
+    <sheet name="Changelog" sheetId="2" r:id="rId4"/>
+    <sheet name="FundTransfer" sheetId="3" state="hidden" r:id="rId5"/>
+    <sheet name="BalenceEnquiry" sheetId="4" state="hidden" r:id="rId6"/>
+    <sheet name="Inter Bank Fund  Transfer" sheetId="5" state="hidden" r:id="rId7"/>
+    <sheet name="Change  password" sheetId="6" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'New Customer'!$A$1:$I$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Unit Testing'!$A$1:$I$64</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="398">
   <si>
     <t>TestCase#</t>
   </si>
@@ -1051,6 +1052,258 @@
   </si>
   <si>
     <t>New Account -Test Cases</t>
+  </si>
+  <si>
+    <t>IP1</t>
+  </si>
+  <si>
+    <t>New Customer</t>
+  </si>
+  <si>
+    <t>Check new Customer is created</t>
+  </si>
+  <si>
+    <t>1) Enter all required fields
+2) Submit</t>
+  </si>
+  <si>
+    <t>Sanjay
+Male
+24/02/1990
+Address - Ahmedabad
+City - Ahmedabad
+State - Gujarat
+PIN - 380009
+Telephone - 8000187025
+Email - sanjayrathod273@gmail.com
+UserId - 1234
+and submit</t>
+  </si>
+  <si>
+    <t>Message Should be display "Customer added successfully !!"</t>
+  </si>
+  <si>
+    <t>IP2</t>
+  </si>
+  <si>
+    <t>Verify Customer is not added twice</t>
+  </si>
+  <si>
+    <t>1) Enter all required field with existing user data
+2) Submit</t>
+  </si>
+  <si>
+    <t>Message Should be displayed"Email address already exist"</t>
+  </si>
+  <si>
+    <t>IP3</t>
+  </si>
+  <si>
+    <t>Edit Customer</t>
+  </si>
+  <si>
+    <t>Check Customer can be edited</t>
+  </si>
+  <si>
+    <t>Message Should be displayed" customer records updated successfully!!"</t>
+  </si>
+  <si>
+    <t>IP4</t>
+  </si>
+  <si>
+    <t>Verify Customer should not be edited for same email id and user id</t>
+  </si>
+  <si>
+    <t>Fill up all fields with repeated email and user id
+for example - Hirenwebdp@gmail.com is associate with userid - 1234
+then for edit other user (name - xyz ) hirenwebdp cannot be associate with user xyz</t>
+  </si>
+  <si>
+    <t>Message Should be display" customer records updated successfully!!"</t>
+  </si>
+  <si>
+    <t>IP5</t>
+  </si>
+  <si>
+    <t>Verify Non existing Customer is not Edited</t>
+  </si>
+  <si>
+    <t>1) Enter the required fields
+2) Submit</t>
+  </si>
+  <si>
+    <t>Customer Id = ABCD</t>
+  </si>
+  <si>
+    <t>Message Should be display" You are not authorise to edit this customer!!"</t>
+  </si>
+  <si>
+    <t>IP6</t>
+  </si>
+  <si>
+    <t>New Account</t>
+  </si>
+  <si>
+    <t>Check New account is added</t>
+  </si>
+  <si>
+    <t>customer id -1234
+account type-saving/current
+Initial Deposit-500</t>
+  </si>
+  <si>
+    <t>Message Should be display " account
+generated successfully"</t>
+  </si>
+  <si>
+    <t>IP7</t>
+  </si>
+  <si>
+    <t>Verify that New Account is not added when same account id already exist</t>
+  </si>
+  <si>
+    <t>1) Enter all fields with customer id and account type already exist</t>
+  </si>
+  <si>
+    <t>IP8</t>
+  </si>
+  <si>
+    <t>Check Ministatement is generated</t>
+  </si>
+  <si>
+    <t>1) Enter Account Number
+2) Submit</t>
+  </si>
+  <si>
+    <t>Account Number - 360560330396</t>
+  </si>
+  <si>
+    <t>Display Generated ministatement</t>
+  </si>
+  <si>
+    <t>IP9</t>
+  </si>
+  <si>
+    <t>Edit Account</t>
+  </si>
+  <si>
+    <t>Check Account is edit</t>
+  </si>
+  <si>
+    <t>1) Enter account number
+2) Submit</t>
+  </si>
+  <si>
+    <t>account number of added account</t>
+  </si>
+  <si>
+    <t>Message Should be display " account
+detail successfully updated"</t>
+  </si>
+  <si>
+    <t>IP10</t>
+  </si>
+  <si>
+    <t>Check Customized Statement is generate</t>
+  </si>
+  <si>
+    <t>IP11</t>
+  </si>
+  <si>
+    <t>Delete Account</t>
+  </si>
+  <si>
+    <t>Verify Account is delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer id -1234
+account type-saving/current
+</t>
+  </si>
+  <si>
+    <t>Message Should be display"Account deleted Successfully"</t>
+  </si>
+  <si>
+    <t>IP12</t>
+  </si>
+  <si>
+    <t>Verify Non Existing Account is not edited</t>
+  </si>
+  <si>
+    <t>Message Should be display"Account does not exist "</t>
+  </si>
+  <si>
+    <t>IP13</t>
+  </si>
+  <si>
+    <t>Verify Non Existing Account is not be deleted</t>
+  </si>
+  <si>
+    <t>IP14</t>
+  </si>
+  <si>
+    <t>Check Ministatement is not generated</t>
+  </si>
+  <si>
+    <t>1)Enter all required field of deleted account
+2)Submit</t>
+  </si>
+  <si>
+    <t>Account number of deleted account</t>
+  </si>
+  <si>
+    <t>Message Should be display - "Account does not exist"</t>
+  </si>
+  <si>
+    <t>IP15</t>
+  </si>
+  <si>
+    <t>Delete customer</t>
+  </si>
+  <si>
+    <t>Verify Customer is Deleted</t>
+  </si>
+  <si>
+    <t>Customer Id - 1234</t>
+  </si>
+  <si>
+    <t>Message Should be display"Customer could not be deleted "</t>
+  </si>
+  <si>
+    <t>IP16</t>
+  </si>
+  <si>
+    <t>Check Customized Statement is not generated</t>
+  </si>
+  <si>
+    <t>Message Should be display"You are not authorise to delete this account "</t>
+  </si>
+  <si>
+    <t>IP17</t>
+  </si>
+  <si>
+    <t>Mini Statement</t>
+  </si>
+  <si>
+    <t>Verify Ministatement is generated</t>
+  </si>
+  <si>
+    <t>Displayed Generated ministatement</t>
+  </si>
+  <si>
+    <t>IP18</t>
+  </si>
+  <si>
+    <t>Customized Statement</t>
+  </si>
+  <si>
+    <t>Check Customized Statement is generated</t>
+  </si>
+  <si>
+    <t>Display Generated Customized statement</t>
+  </si>
+  <si>
+    <t>Failure</t>
   </si>
 </sst>
 </file>
@@ -1084,10 +1337,12 @@
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1153,7 +1408,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1508,11 +1763,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1570,36 +1942,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1608,15 +1950,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1630,7 +1963,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1648,15 +1981,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1668,15 +1992,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1732,16 +2047,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1749,6 +2058,123 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2369,7 +2795,7 @@
   <dimension ref="A1:Y102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
@@ -2386,34 +2812,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13.5" thickBot="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="G1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="H1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="J1" s="35"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
       <c r="M1" s="16"/>
@@ -2428,10 +2854,10 @@
       <c r="V1" s="16"/>
     </row>
     <row r="2" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="75" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="16" t="s">
@@ -2450,8 +2876,8 @@
       <c r="H2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="35"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="22"/>
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
       <c r="M2" s="16"/>
@@ -2469,10 +2895,10 @@
       <c r="Y2" s="13"/>
     </row>
     <row r="3" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="25"/>
+      <c r="B3" s="76"/>
       <c r="C3" s="16" t="s">
         <v>108</v>
       </c>
@@ -2489,8 +2915,8 @@
       <c r="H3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="35"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="22"/>
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
       <c r="M3" s="16"/>
@@ -2508,10 +2934,10 @@
       <c r="Y3" s="13"/>
     </row>
     <row r="4" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="76"/>
       <c r="C4" s="16" t="s">
         <v>112</v>
       </c>
@@ -2528,8 +2954,8 @@
       <c r="H4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="59"/>
-      <c r="J4" s="35"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="22"/>
       <c r="K4" s="16"/>
       <c r="L4" s="16"/>
       <c r="M4" s="16"/>
@@ -2547,10 +2973,10 @@
       <c r="Y4" s="13"/>
     </row>
     <row r="5" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="17" t="s">
         <v>116</v>
       </c>
@@ -2567,8 +2993,8 @@
       <c r="H5" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="I5" s="61"/>
-      <c r="J5" s="36"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="23"/>
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
@@ -2586,10 +3012,10 @@
       <c r="Y5" s="13"/>
     </row>
     <row r="6" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="78" t="s">
         <v>119</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -2608,8 +3034,8 @@
       <c r="H6" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="I6" s="61"/>
-      <c r="J6" s="36"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="23"/>
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
@@ -2627,10 +3053,10 @@
       <c r="Y6" s="13"/>
     </row>
     <row r="7" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="17" t="s">
         <v>124</v>
       </c>
@@ -2647,8 +3073,8 @@
       <c r="H7" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="I7" s="61"/>
-      <c r="J7" s="36"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="23"/>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
@@ -2666,10 +3092,10 @@
       <c r="Y7" s="13"/>
     </row>
     <row r="8" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="75" t="s">
         <v>126</v>
       </c>
       <c r="C8" s="16" t="s">
@@ -2686,8 +3112,8 @@
       <c r="H8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="59"/>
-      <c r="J8" s="35"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="22"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
@@ -2705,10 +3131,10 @@
       <c r="Y8" s="13"/>
     </row>
     <row r="9" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="25"/>
+      <c r="B9" s="76"/>
       <c r="C9" s="16" t="s">
         <v>131</v>
       </c>
@@ -2725,8 +3151,8 @@
       <c r="H9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="59"/>
-      <c r="J9" s="35"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="22"/>
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
@@ -2744,10 +3170,10 @@
       <c r="Y9" s="13"/>
     </row>
     <row r="10" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="B10" s="25"/>
+      <c r="B10" s="76"/>
       <c r="C10" s="16" t="s">
         <v>135</v>
       </c>
@@ -2764,8 +3190,8 @@
       <c r="H10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="59"/>
-      <c r="J10" s="35"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="22"/>
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
       <c r="M10" s="16"/>
@@ -2783,10 +3209,10 @@
       <c r="Y10" s="13"/>
     </row>
     <row r="11" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="77"/>
       <c r="C11" s="17" t="s">
         <v>139</v>
       </c>
@@ -2803,8 +3229,8 @@
       <c r="H11" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="I11" s="61"/>
-      <c r="J11" s="36"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="23"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
@@ -2822,10 +3248,10 @@
       <c r="Y11" s="13"/>
     </row>
     <row r="12" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="75" t="s">
         <v>141</v>
       </c>
       <c r="C12" s="16" t="s">
@@ -2842,8 +3268,8 @@
       <c r="H12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="59"/>
-      <c r="J12" s="35"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="22"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
@@ -2861,10 +3287,10 @@
       <c r="Y12" s="13"/>
     </row>
     <row r="13" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="B13" s="25"/>
+      <c r="B13" s="76"/>
       <c r="C13" s="16" t="s">
         <v>146</v>
       </c>
@@ -2881,8 +3307,8 @@
       <c r="H13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="59"/>
-      <c r="J13" s="35"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="22"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
@@ -2900,10 +3326,10 @@
       <c r="Y13" s="13"/>
     </row>
     <row r="14" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="B14" s="25"/>
+      <c r="B14" s="76"/>
       <c r="C14" s="16" t="s">
         <v>150</v>
       </c>
@@ -2920,8 +3346,8 @@
       <c r="H14" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="59"/>
-      <c r="J14" s="35"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="22"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
@@ -2939,10 +3365,10 @@
       <c r="Y14" s="13"/>
     </row>
     <row r="15" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="B15" s="26"/>
+      <c r="B15" s="77"/>
       <c r="C15" s="17" t="s">
         <v>154</v>
       </c>
@@ -2959,8 +3385,8 @@
       <c r="H15" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="I15" s="61"/>
-      <c r="J15" s="36"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="23"/>
       <c r="K15" s="17"/>
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
@@ -2978,10 +3404,10 @@
       <c r="Y15" s="13"/>
     </row>
     <row r="16" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="75" t="s">
         <v>156</v>
       </c>
       <c r="C16" s="16" t="s">
@@ -3000,8 +3426,8 @@
       <c r="H16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="59"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="22"/>
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
@@ -3019,10 +3445,10 @@
       <c r="Y16" s="13"/>
     </row>
     <row r="17" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="B17" s="25"/>
+      <c r="B17" s="76"/>
       <c r="C17" s="16" t="s">
         <v>162</v>
       </c>
@@ -3037,8 +3463,8 @@
       <c r="H17" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="59"/>
-      <c r="J17" s="35"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="22"/>
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
@@ -3056,10 +3482,10 @@
       <c r="Y17" s="13"/>
     </row>
     <row r="18" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="B18" s="25"/>
+      <c r="B18" s="76"/>
       <c r="C18" s="16" t="s">
         <v>166</v>
       </c>
@@ -3076,8 +3502,8 @@
       <c r="H18" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="59"/>
-      <c r="J18" s="35"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="22"/>
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
       <c r="M18" s="16"/>
@@ -3095,10 +3521,10 @@
       <c r="Y18" s="13"/>
     </row>
     <row r="19" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="B19" s="25"/>
+      <c r="B19" s="76"/>
       <c r="C19" s="16" t="s">
         <v>171</v>
       </c>
@@ -3115,8 +3541,8 @@
       <c r="H19" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="59"/>
-      <c r="J19" s="35"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="22"/>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
@@ -3134,10 +3560,10 @@
       <c r="Y19" s="13"/>
     </row>
     <row r="20" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="B20" s="25"/>
+      <c r="B20" s="76"/>
       <c r="C20" s="17" t="s">
         <v>175</v>
       </c>
@@ -3151,11 +3577,11 @@
       <c r="G20" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="H20" s="39" t="s">
+      <c r="H20" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="I20" s="61"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="23"/>
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
@@ -3173,10 +3599,10 @@
       <c r="Y20" s="13"/>
     </row>
     <row r="21" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A21" s="60" t="s">
+      <c r="A21" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="B21" s="26"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="17" t="s">
         <v>177</v>
       </c>
@@ -3193,8 +3619,8 @@
       <c r="H21" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="I21" s="61"/>
-      <c r="J21" s="36"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="23"/>
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
       <c r="M21" s="17"/>
@@ -3212,10 +3638,10 @@
       <c r="Y21" s="13"/>
     </row>
     <row r="22" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="75" t="s">
         <v>180</v>
       </c>
       <c r="C22" s="16" t="s">
@@ -3232,8 +3658,8 @@
       <c r="H22" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="59"/>
-      <c r="J22" s="35"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="22"/>
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
       <c r="M22" s="16"/>
@@ -3251,10 +3677,10 @@
       <c r="Y22" s="13"/>
     </row>
     <row r="23" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="B23" s="25"/>
+      <c r="B23" s="76"/>
       <c r="C23" s="17" t="s">
         <v>185</v>
       </c>
@@ -3271,8 +3697,8 @@
       <c r="H23" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="I23" s="61"/>
-      <c r="J23" s="36"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="23"/>
       <c r="K23" s="17"/>
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
@@ -3290,10 +3716,10 @@
       <c r="Y23" s="13"/>
     </row>
     <row r="24" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A24" s="60" t="s">
+      <c r="A24" s="41" t="s">
         <v>186</v>
       </c>
-      <c r="B24" s="25"/>
+      <c r="B24" s="76"/>
       <c r="C24" s="17" t="s">
         <v>187</v>
       </c>
@@ -3312,8 +3738,8 @@
       <c r="H24" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="I24" s="61"/>
-      <c r="J24" s="36"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="23"/>
       <c r="K24" s="17"/>
       <c r="L24" s="17"/>
       <c r="M24" s="17"/>
@@ -3331,10 +3757,10 @@
       <c r="Y24" s="13"/>
     </row>
     <row r="25" spans="1:25" ht="39" thickBot="1">
-      <c r="A25" s="58" t="s">
+      <c r="A25" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="B25" s="26"/>
+      <c r="B25" s="77"/>
       <c r="C25" s="16" t="s">
         <v>192</v>
       </c>
@@ -3351,8 +3777,8 @@
       <c r="H25" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="59"/>
-      <c r="J25" s="35"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="22"/>
       <c r="K25" s="16"/>
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
@@ -3370,10 +3796,10 @@
       <c r="Y25" s="13"/>
     </row>
     <row r="26" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="75" t="s">
         <v>196</v>
       </c>
       <c r="C26" s="16" t="s">
@@ -3390,8 +3816,8 @@
       <c r="H26" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="59"/>
-      <c r="J26" s="35"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="22"/>
       <c r="K26" s="16"/>
       <c r="L26" s="16"/>
       <c r="M26" s="16"/>
@@ -3409,10 +3835,10 @@
       <c r="Y26" s="13"/>
     </row>
     <row r="27" spans="1:25" ht="77.25" thickBot="1">
-      <c r="A27" s="58" t="s">
+      <c r="A27" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="B27" s="25"/>
+      <c r="B27" s="76"/>
       <c r="C27" s="16" t="s">
         <v>201</v>
       </c>
@@ -3429,8 +3855,8 @@
       <c r="H27" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="59"/>
-      <c r="J27" s="35"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="22"/>
       <c r="K27" s="16"/>
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
@@ -3448,10 +3874,10 @@
       <c r="Y27" s="13"/>
     </row>
     <row r="28" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A28" s="60" t="s">
+      <c r="A28" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="B28" s="26"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="17" t="s">
         <v>206</v>
       </c>
@@ -3468,8 +3894,8 @@
       <c r="H28" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="I28" s="61"/>
-      <c r="J28" s="36"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="23"/>
       <c r="K28" s="17"/>
       <c r="L28" s="17"/>
       <c r="M28" s="17"/>
@@ -3487,30 +3913,30 @@
       <c r="Y28" s="13"/>
     </row>
     <row r="29" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A29" s="62" t="s">
+      <c r="A29" s="43" t="s">
         <v>209</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="C29" s="40" t="s">
+      <c r="C29" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40" t="s">
+      <c r="E29" s="27"/>
+      <c r="F29" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="G29" s="41" t="s">
+      <c r="G29" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="H29" s="42" t="s">
+      <c r="H29" s="29" t="s">
         <v>217</v>
       </c>
-      <c r="I29" s="63"/>
-      <c r="J29" s="35"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="22"/>
       <c r="K29" s="16"/>
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
@@ -3528,18 +3954,18 @@
       <c r="Y29" s="13"/>
     </row>
     <row r="30" spans="1:25" ht="39" customHeight="1" thickBot="1">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="80" t="s">
         <v>281</v>
       </c>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="35"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="81"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="82"/>
+      <c r="J30" s="22"/>
       <c r="K30" s="16"/>
       <c r="L30" s="16"/>
       <c r="M30" s="16"/>
@@ -3557,30 +3983,30 @@
       <c r="Y30" s="13"/>
     </row>
     <row r="31" spans="1:25" ht="39" thickBot="1">
-      <c r="A31" s="64" t="s">
+      <c r="A31" s="45" t="s">
         <v>224</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="86" t="s">
         <v>225</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="D31" s="43" t="s">
+      <c r="D31" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="E31" s="38"/>
-      <c r="F31" s="43" t="s">
+      <c r="E31" s="25"/>
+      <c r="F31" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="G31" s="44" t="s">
+      <c r="G31" s="31" t="s">
         <v>282</v>
       </c>
-      <c r="H31" s="44" t="s">
+      <c r="H31" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="I31" s="65"/>
-      <c r="J31" s="35"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="22"/>
       <c r="K31" s="16"/>
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
@@ -3598,30 +4024,30 @@
       <c r="Y31" s="13"/>
     </row>
     <row r="32" spans="1:25" ht="26.25" thickBot="1">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="47" t="s">
         <v>229</v>
       </c>
-      <c r="B32" s="20"/>
+      <c r="B32" s="86"/>
       <c r="C32" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E32" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="F32" s="29" t="s">
+      <c r="F32" s="19" t="s">
         <v>160</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H32" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="I32" s="65"/>
-      <c r="J32" s="35"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="22"/>
       <c r="K32" s="16"/>
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
@@ -3639,30 +4065,30 @@
       <c r="Y32" s="13"/>
     </row>
     <row r="33" spans="1:25" ht="39" thickBot="1">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="B33" s="20"/>
+      <c r="B33" s="86"/>
       <c r="C33" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="D33" s="29" t="s">
+      <c r="D33" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="E33" s="29" t="s">
+      <c r="E33" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="29" t="s">
+      <c r="F33" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="G33" s="29" t="s">
+      <c r="G33" s="19" t="s">
         <v>284</v>
       </c>
       <c r="H33" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="65"/>
-      <c r="J33" s="35"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="22"/>
       <c r="K33" s="16"/>
       <c r="L33" s="16"/>
       <c r="M33" s="16"/>
@@ -3680,30 +4106,30 @@
       <c r="Y33" s="13"/>
     </row>
     <row r="34" spans="1:25" ht="39" thickBot="1">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="B34" s="21"/>
+      <c r="B34" s="87"/>
       <c r="C34" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="D34" s="29" t="s">
+      <c r="D34" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="E34" s="29" t="s">
+      <c r="E34" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="F34" s="29" t="s">
+      <c r="F34" s="19" t="s">
         <v>240</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H34" s="17" t="s">
+      <c r="H34" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="I34" s="65"/>
-      <c r="J34" s="35"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="22"/>
       <c r="K34" s="16"/>
       <c r="L34" s="16"/>
       <c r="M34" s="16"/>
@@ -3721,30 +4147,30 @@
       <c r="Y34" s="13"/>
     </row>
     <row r="35" spans="1:25" ht="39" thickBot="1">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="47" t="s">
         <v>241</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="29" t="s">
+      <c r="D35" s="19" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="16"/>
-      <c r="F35" s="29" t="s">
+      <c r="F35" s="19" t="s">
         <v>242</v>
       </c>
       <c r="G35" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I35" s="65"/>
-      <c r="J35" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I35" s="46"/>
+      <c r="J35" s="22"/>
       <c r="K35" s="16"/>
       <c r="L35" s="16"/>
       <c r="M35" s="16"/>
@@ -3762,30 +4188,30 @@
       <c r="Y35" s="13"/>
     </row>
     <row r="36" spans="1:25" ht="39" thickBot="1">
-      <c r="A36" s="66" t="s">
+      <c r="A36" s="47" t="s">
         <v>243</v>
       </c>
-      <c r="B36" s="33"/>
-      <c r="C36" s="29" t="s">
+      <c r="B36" s="91"/>
+      <c r="C36" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="E36" s="29" t="s">
+      <c r="E36" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F36" s="29" t="s">
+      <c r="F36" s="19" t="s">
         <v>244</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I36" s="65"/>
-      <c r="J36" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I36" s="46"/>
+      <c r="J36" s="22"/>
       <c r="K36" s="16"/>
       <c r="L36" s="16"/>
       <c r="M36" s="16"/>
@@ -3803,30 +4229,30 @@
       <c r="Y36" s="13"/>
     </row>
     <row r="37" spans="1:25" ht="39" thickBot="1">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="47" t="s">
         <v>245</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="29" t="s">
+      <c r="B37" s="92"/>
+      <c r="C37" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E37" s="29" t="s">
+      <c r="E37" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="29" t="s">
+      <c r="F37" s="19" t="s">
         <v>247</v>
       </c>
       <c r="G37" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I37" s="65"/>
-      <c r="J37" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I37" s="46"/>
+      <c r="J37" s="22"/>
       <c r="K37" s="16"/>
       <c r="L37" s="16"/>
       <c r="M37" s="16"/>
@@ -3844,30 +4270,30 @@
       <c r="Y37" s="13"/>
     </row>
     <row r="38" spans="1:25" ht="39" thickBot="1">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="47" t="s">
         <v>248</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="C38" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="19" t="s">
         <v>121</v>
       </c>
       <c r="E38" s="16"/>
-      <c r="F38" s="29" t="s">
+      <c r="F38" s="19" t="s">
         <v>122</v>
       </c>
       <c r="G38" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I38" s="65"/>
-      <c r="J38" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I38" s="46"/>
+      <c r="J38" s="22"/>
       <c r="K38" s="16"/>
       <c r="L38" s="16"/>
       <c r="M38" s="16"/>
@@ -3882,30 +4308,30 @@
       <c r="V38" s="16"/>
     </row>
     <row r="39" spans="1:25" ht="39" thickBot="1">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="47" t="s">
         <v>249</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="90" t="s">
         <v>126</v>
       </c>
-      <c r="C39" s="29" t="s">
+      <c r="C39" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="D39" s="19" t="s">
         <v>128</v>
       </c>
       <c r="E39" s="16"/>
-      <c r="F39" s="29" t="s">
+      <c r="F39" s="19" t="s">
         <v>250</v>
       </c>
       <c r="G39" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I39" s="65"/>
-      <c r="J39" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I39" s="46"/>
+      <c r="J39" s="22"/>
       <c r="K39" s="16"/>
       <c r="L39" s="16"/>
       <c r="M39" s="16"/>
@@ -3920,30 +4346,30 @@
       <c r="V39" s="16"/>
     </row>
     <row r="40" spans="1:25" ht="39" thickBot="1">
-      <c r="A40" s="66" t="s">
+      <c r="A40" s="47" t="s">
         <v>251</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="29" t="s">
+      <c r="B40" s="91"/>
+      <c r="C40" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="D40" s="29" t="s">
+      <c r="D40" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E40" s="29" t="s">
+      <c r="E40" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="F40" s="29" t="s">
+      <c r="F40" s="19" t="s">
         <v>252</v>
       </c>
       <c r="G40" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I40" s="65"/>
-      <c r="J40" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I40" s="46"/>
+      <c r="J40" s="22"/>
       <c r="K40" s="16"/>
       <c r="L40" s="16"/>
       <c r="M40" s="16"/>
@@ -3958,30 +4384,30 @@
       <c r="V40" s="16"/>
     </row>
     <row r="41" spans="1:25" ht="39" thickBot="1">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="47" t="s">
         <v>253</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="29" t="s">
+      <c r="B41" s="92"/>
+      <c r="C41" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="D41" s="29" t="s">
+      <c r="D41" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="E41" s="29" t="s">
+      <c r="E41" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="F41" s="29" t="s">
+      <c r="F41" s="19" t="s">
         <v>254</v>
       </c>
       <c r="G41" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I41" s="65"/>
-      <c r="J41" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I41" s="46"/>
+      <c r="J41" s="22"/>
       <c r="K41" s="16"/>
       <c r="L41" s="16"/>
       <c r="M41" s="16"/>
@@ -3996,30 +4422,30 @@
       <c r="V41" s="16"/>
     </row>
     <row r="42" spans="1:25" ht="39" thickBot="1">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="47" t="s">
         <v>255</v>
       </c>
-      <c r="B42" s="32" t="s">
+      <c r="B42" s="90" t="s">
         <v>141</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C42" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="D42" s="29" t="s">
+      <c r="D42" s="19" t="s">
         <v>143</v>
       </c>
       <c r="E42" s="16"/>
-      <c r="F42" s="29" t="s">
+      <c r="F42" s="19" t="s">
         <v>257</v>
       </c>
       <c r="G42" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I42" s="65"/>
-      <c r="J42" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I42" s="46"/>
+      <c r="J42" s="22"/>
       <c r="K42" s="16"/>
       <c r="L42" s="16"/>
       <c r="M42" s="16"/>
@@ -4034,30 +4460,30 @@
       <c r="V42" s="16"/>
     </row>
     <row r="43" spans="1:25" ht="39" thickBot="1">
-      <c r="A43" s="66" t="s">
+      <c r="A43" s="47" t="s">
         <v>258</v>
       </c>
-      <c r="B43" s="33"/>
-      <c r="C43" s="29" t="s">
+      <c r="B43" s="91"/>
+      <c r="C43" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D43" s="29" t="s">
+      <c r="D43" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="E43" s="29" t="s">
+      <c r="E43" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="F43" s="29" t="s">
+      <c r="F43" s="19" t="s">
         <v>111</v>
       </c>
       <c r="G43" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I43" s="65"/>
-      <c r="J43" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I43" s="46"/>
+      <c r="J43" s="22"/>
       <c r="K43" s="16"/>
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
@@ -4072,30 +4498,30 @@
       <c r="V43" s="16"/>
     </row>
     <row r="44" spans="1:25" ht="39" thickBot="1">
-      <c r="A44" s="66" t="s">
+      <c r="A44" s="47" t="s">
         <v>259</v>
       </c>
-      <c r="B44" s="34"/>
-      <c r="C44" s="29" t="s">
+      <c r="B44" s="92"/>
+      <c r="C44" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="D44" s="29" t="s">
+      <c r="D44" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E44" s="29" t="s">
+      <c r="E44" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="F44" s="29" t="s">
+      <c r="F44" s="19" t="s">
         <v>254</v>
       </c>
       <c r="G44" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I44" s="65"/>
-      <c r="J44" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I44" s="46"/>
+      <c r="J44" s="22"/>
       <c r="K44" s="16"/>
       <c r="L44" s="16"/>
       <c r="M44" s="16"/>
@@ -4110,32 +4536,32 @@
       <c r="V44" s="16"/>
     </row>
     <row r="45" spans="1:25" ht="39" thickBot="1">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="47" t="s">
         <v>260</v>
       </c>
-      <c r="B45" s="32" t="s">
+      <c r="B45" s="90" t="s">
         <v>156</v>
       </c>
-      <c r="C45" s="29" t="s">
+      <c r="C45" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="D45" s="29" t="s">
+      <c r="D45" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="E45" s="29" t="s">
+      <c r="E45" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="F45" s="29" t="s">
+      <c r="F45" s="19" t="s">
         <v>261</v>
       </c>
       <c r="G45" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H45" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I45" s="65"/>
-      <c r="J45" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I45" s="46"/>
+      <c r="J45" s="22"/>
       <c r="K45" s="16"/>
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
@@ -4150,28 +4576,28 @@
       <c r="V45" s="16"/>
     </row>
     <row r="46" spans="1:25" ht="39" thickBot="1">
-      <c r="A46" s="66" t="s">
+      <c r="A46" s="47" t="s">
         <v>262</v>
       </c>
-      <c r="B46" s="33"/>
-      <c r="C46" s="29" t="s">
+      <c r="B46" s="91"/>
+      <c r="C46" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="D46" s="29" t="s">
+      <c r="D46" s="19" t="s">
         <v>163</v>
       </c>
       <c r="E46" s="16"/>
-      <c r="F46" s="29" t="s">
+      <c r="F46" s="19" t="s">
         <v>263</v>
       </c>
       <c r="G46" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I46" s="65"/>
-      <c r="J46" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I46" s="46"/>
+      <c r="J46" s="22"/>
       <c r="K46" s="16"/>
       <c r="L46" s="16"/>
       <c r="M46" s="16"/>
@@ -4186,30 +4612,30 @@
       <c r="V46" s="16"/>
     </row>
     <row r="47" spans="1:25" ht="51.75" thickBot="1">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="47" t="s">
         <v>264</v>
       </c>
-      <c r="B47" s="33"/>
-      <c r="C47" s="29" t="s">
+      <c r="B47" s="91"/>
+      <c r="C47" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="D47" s="29" t="s">
+      <c r="D47" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="E47" s="29" t="s">
+      <c r="E47" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="F47" s="29" t="s">
+      <c r="F47" s="19" t="s">
         <v>266</v>
       </c>
       <c r="G47" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I47" s="65"/>
-      <c r="J47" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I47" s="46"/>
+      <c r="J47" s="22"/>
       <c r="K47" s="16"/>
       <c r="L47" s="16"/>
       <c r="M47" s="16"/>
@@ -4224,30 +4650,30 @@
       <c r="V47" s="16"/>
     </row>
     <row r="48" spans="1:25" ht="39" thickBot="1">
-      <c r="A48" s="66" t="s">
+      <c r="A48" s="47" t="s">
         <v>267</v>
       </c>
-      <c r="B48" s="34"/>
-      <c r="C48" s="29" t="s">
+      <c r="B48" s="92"/>
+      <c r="C48" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="D48" s="29" t="s">
+      <c r="D48" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="E48" s="29" t="s">
+      <c r="E48" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="F48" s="29" t="s">
+      <c r="F48" s="19" t="s">
         <v>268</v>
       </c>
       <c r="G48" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I48" s="65"/>
-      <c r="J48" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I48" s="46"/>
+      <c r="J48" s="22"/>
       <c r="K48" s="16"/>
       <c r="L48" s="16"/>
       <c r="M48" s="16"/>
@@ -4262,30 +4688,30 @@
       <c r="V48" s="16"/>
     </row>
     <row r="49" spans="1:22" ht="39" thickBot="1">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="B49" s="32" t="s">
+      <c r="B49" s="90" t="s">
         <v>180</v>
       </c>
-      <c r="C49" s="29" t="s">
+      <c r="C49" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="D49" s="29" t="s">
+      <c r="D49" s="19" t="s">
         <v>182</v>
       </c>
       <c r="E49" s="16"/>
-      <c r="F49" s="29" t="s">
+      <c r="F49" s="19" t="s">
         <v>270</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I49" s="65"/>
-      <c r="J49" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I49" s="46"/>
+      <c r="J49" s="22"/>
       <c r="K49" s="16"/>
       <c r="L49" s="16"/>
       <c r="M49" s="16"/>
@@ -4300,30 +4726,30 @@
       <c r="V49" s="16"/>
     </row>
     <row r="50" spans="1:22" ht="39" thickBot="1">
-      <c r="A50" s="66" t="s">
+      <c r="A50" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="B50" s="34"/>
-      <c r="C50" s="29" t="s">
+      <c r="B50" s="92"/>
+      <c r="C50" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="D50" s="29" t="s">
+      <c r="D50" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="E50" s="29" t="s">
+      <c r="E50" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="F50" s="29" t="s">
+      <c r="F50" s="19" t="s">
         <v>272</v>
       </c>
       <c r="G50" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I50" s="65"/>
-      <c r="J50" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I50" s="46"/>
+      <c r="J50" s="22"/>
       <c r="K50" s="16"/>
       <c r="L50" s="16"/>
       <c r="M50" s="16"/>
@@ -4338,30 +4764,30 @@
       <c r="V50" s="16"/>
     </row>
     <row r="51" spans="1:22" ht="39" thickBot="1">
-      <c r="A51" s="66" t="s">
+      <c r="A51" s="47" t="s">
         <v>273</v>
       </c>
-      <c r="B51" s="32" t="s">
+      <c r="B51" s="90" t="s">
         <v>196</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="D51" s="19" t="s">
         <v>198</v>
       </c>
       <c r="E51" s="16"/>
-      <c r="F51" s="29" t="s">
+      <c r="F51" s="19" t="s">
         <v>274</v>
       </c>
       <c r="G51" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H51" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I51" s="65"/>
-      <c r="J51" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I51" s="46"/>
+      <c r="J51" s="22"/>
       <c r="K51" s="16"/>
       <c r="L51" s="16"/>
       <c r="M51" s="16"/>
@@ -4376,30 +4802,30 @@
       <c r="V51" s="16"/>
     </row>
     <row r="52" spans="1:22" ht="64.5" thickBot="1">
-      <c r="A52" s="66" t="s">
+      <c r="A52" s="47" t="s">
         <v>275</v>
       </c>
-      <c r="B52" s="33"/>
-      <c r="C52" s="29" t="s">
+      <c r="B52" s="91"/>
+      <c r="C52" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="D52" s="29" t="s">
+      <c r="D52" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="E52" s="29" t="s">
+      <c r="E52" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="F52" s="29" t="s">
+      <c r="F52" s="19" t="s">
         <v>278</v>
       </c>
       <c r="G52" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H52" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="I52" s="65"/>
-      <c r="J52" s="35"/>
+        <v>397</v>
+      </c>
+      <c r="I52" s="46"/>
+      <c r="J52" s="22"/>
       <c r="K52" s="16"/>
       <c r="L52" s="16"/>
       <c r="M52" s="16"/>
@@ -4414,30 +4840,30 @@
       <c r="V52" s="16"/>
     </row>
     <row r="53" spans="1:22" ht="77.25" thickBot="1">
-      <c r="A53" s="67" t="s">
+      <c r="A53" s="48" t="s">
         <v>279</v>
       </c>
-      <c r="B53" s="33"/>
-      <c r="C53" s="40" t="s">
+      <c r="B53" s="91"/>
+      <c r="C53" s="27" t="s">
         <v>276</v>
       </c>
-      <c r="D53" s="48" t="s">
+      <c r="D53" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="E53" s="48" t="s">
+      <c r="E53" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="F53" s="48" t="s">
+      <c r="F53" s="32" t="s">
         <v>280</v>
       </c>
-      <c r="G53" s="41" t="s">
+      <c r="G53" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="H53" s="41" t="s">
-        <v>217</v>
-      </c>
-      <c r="I53" s="65"/>
-      <c r="J53" s="35"/>
+      <c r="H53" s="17" t="s">
+        <v>397</v>
+      </c>
+      <c r="I53" s="46"/>
+      <c r="J53" s="22"/>
       <c r="K53" s="16"/>
       <c r="L53" s="16"/>
       <c r="M53" s="16"/>
@@ -4452,18 +4878,18 @@
       <c r="V53" s="16"/>
     </row>
     <row r="54" spans="1:22" ht="39" customHeight="1" thickBot="1">
-      <c r="A54" s="52" t="s">
+      <c r="A54" s="83" t="s">
         <v>321</v>
       </c>
-      <c r="B54" s="53"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="53"/>
-      <c r="E54" s="53"/>
-      <c r="F54" s="53"/>
-      <c r="G54" s="53"/>
-      <c r="H54" s="53"/>
-      <c r="I54" s="54"/>
-      <c r="J54" s="35"/>
+      <c r="B54" s="84"/>
+      <c r="C54" s="84"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="84"/>
+      <c r="F54" s="84"/>
+      <c r="G54" s="84"/>
+      <c r="H54" s="84"/>
+      <c r="I54" s="85"/>
+      <c r="J54" s="22"/>
       <c r="K54" s="16"/>
       <c r="L54" s="16"/>
       <c r="M54" s="16"/>
@@ -4478,31 +4904,31 @@
       <c r="V54" s="16"/>
     </row>
     <row r="55" spans="1:22" ht="39" thickBot="1">
-      <c r="A55" s="68" t="s">
+      <c r="A55" s="49" t="s">
         <v>287</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="86" t="s">
         <v>225</v>
       </c>
-      <c r="C55" s="49" t="s">
+      <c r="C55" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="D55" s="50" t="s">
+      <c r="D55" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="E55" s="49"/>
-      <c r="F55" s="50" t="s">
+      <c r="E55" s="33"/>
+      <c r="F55" s="34" t="s">
         <v>288</v>
       </c>
-      <c r="G55" s="41" t="s">
+      <c r="G55" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="H55" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="I55" s="69"/>
-      <c r="J55" s="37"/>
-      <c r="K55" s="30"/>
+      <c r="H55" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="I55" s="50"/>
+      <c r="J55" s="24"/>
+      <c r="K55" s="20"/>
       <c r="L55" s="16"/>
       <c r="M55" s="16"/>
       <c r="N55" s="16"/>
@@ -4516,31 +4942,31 @@
       <c r="V55" s="16"/>
     </row>
     <row r="56" spans="1:22" ht="39" thickBot="1">
-      <c r="A56" s="70" t="s">
+      <c r="A56" s="51" t="s">
         <v>289</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="30" t="s">
+      <c r="B56" s="86"/>
+      <c r="C56" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="D56" s="31" t="s">
+      <c r="D56" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="E56" s="31" t="s">
+      <c r="E56" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="F56" s="31" t="s">
+      <c r="F56" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="G56" s="41" t="s">
+      <c r="G56" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="H56" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="I56" s="71"/>
-      <c r="J56" s="37"/>
-      <c r="K56" s="30"/>
+      <c r="H56" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="I56" s="52"/>
+      <c r="J56" s="24"/>
+      <c r="K56" s="20"/>
       <c r="L56" s="16"/>
       <c r="M56" s="16"/>
       <c r="N56" s="16"/>
@@ -4554,31 +4980,31 @@
       <c r="V56" s="16"/>
     </row>
     <row r="57" spans="1:22" ht="39" thickBot="1">
-      <c r="A57" s="70" t="s">
+      <c r="A57" s="51" t="s">
         <v>291</v>
       </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="30" t="s">
+      <c r="B57" s="86"/>
+      <c r="C57" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="D57" s="31" t="s">
+      <c r="D57" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="E57" s="31" t="s">
+      <c r="E57" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="F57" s="31" t="s">
+      <c r="F57" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="G57" s="41" t="s">
+      <c r="G57" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="H57" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="I57" s="71"/>
-      <c r="J57" s="37"/>
-      <c r="K57" s="30"/>
+      <c r="H57" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="I57" s="52"/>
+      <c r="J57" s="24"/>
+      <c r="K57" s="20"/>
       <c r="L57" s="16"/>
       <c r="M57" s="16"/>
       <c r="N57" s="16"/>
@@ -4592,31 +5018,31 @@
       <c r="V57" s="16"/>
     </row>
     <row r="58" spans="1:22" ht="39" thickBot="1">
-      <c r="A58" s="70" t="s">
+      <c r="A58" s="51" t="s">
         <v>293</v>
       </c>
-      <c r="B58" s="20"/>
-      <c r="C58" s="30" t="s">
+      <c r="B58" s="86"/>
+      <c r="C58" s="20" t="s">
         <v>294</v>
       </c>
-      <c r="D58" s="31" t="s">
+      <c r="D58" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="E58" s="30" t="s">
+      <c r="E58" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="F58" s="31" t="s">
+      <c r="F58" s="21" t="s">
         <v>297</v>
       </c>
-      <c r="G58" s="41" t="s">
+      <c r="G58" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="H58" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="I58" s="71"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="30"/>
+      <c r="H58" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="I58" s="52"/>
+      <c r="J58" s="24"/>
+      <c r="K58" s="20"/>
       <c r="L58" s="16"/>
       <c r="M58" s="16"/>
       <c r="N58" s="16"/>
@@ -4630,29 +5056,29 @@
       <c r="V58" s="16"/>
     </row>
     <row r="59" spans="1:22" ht="39" thickBot="1">
-      <c r="A59" s="70" t="s">
+      <c r="A59" s="51" t="s">
         <v>298</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="30" t="s">
+      <c r="B59" s="87"/>
+      <c r="C59" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="D59" s="31" t="s">
+      <c r="D59" s="21" t="s">
         <v>300</v>
       </c>
-      <c r="E59" s="30"/>
-      <c r="F59" s="31" t="s">
+      <c r="E59" s="20"/>
+      <c r="F59" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="G59" s="41" t="s">
+      <c r="G59" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="H59" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="I59" s="71"/>
-      <c r="J59" s="37"/>
-      <c r="K59" s="30"/>
+      <c r="H59" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="I59" s="52"/>
+      <c r="J59" s="24"/>
+      <c r="K59" s="20"/>
       <c r="L59" s="16"/>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
@@ -4666,31 +5092,31 @@
       <c r="V59" s="16"/>
     </row>
     <row r="60" spans="1:22" ht="39" thickBot="1">
-      <c r="A60" s="70" t="s">
+      <c r="A60" s="51" t="s">
         <v>302</v>
       </c>
-      <c r="B60" s="19" t="s">
+      <c r="B60" s="88" t="s">
         <v>303</v>
       </c>
-      <c r="C60" s="30" t="s">
+      <c r="C60" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="D60" s="31" t="s">
+      <c r="D60" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="E60" s="30"/>
-      <c r="F60" s="31" t="s">
+      <c r="E60" s="20"/>
+      <c r="F60" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="G60" s="41" t="s">
+      <c r="G60" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="H60" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="I60" s="71"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="30"/>
+      <c r="H60" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="I60" s="52"/>
+      <c r="J60" s="24"/>
+      <c r="K60" s="20"/>
       <c r="L60" s="16"/>
       <c r="M60" s="16"/>
       <c r="N60" s="16"/>
@@ -4704,31 +5130,31 @@
       <c r="V60" s="16"/>
     </row>
     <row r="61" spans="1:22" ht="39" thickBot="1">
-      <c r="A61" s="70" t="s">
+      <c r="A61" s="51" t="s">
         <v>307</v>
       </c>
-      <c r="B61" s="20"/>
-      <c r="C61" s="30" t="s">
+      <c r="B61" s="86"/>
+      <c r="C61" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="D61" s="31" t="s">
+      <c r="D61" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="E61" s="31" t="s">
+      <c r="E61" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="F61" s="31" t="s">
+      <c r="F61" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="G61" s="41" t="s">
+      <c r="G61" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="H61" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="I61" s="71"/>
-      <c r="J61" s="37"/>
-      <c r="K61" s="30"/>
+      <c r="H61" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="I61" s="52"/>
+      <c r="J61" s="24"/>
+      <c r="K61" s="20"/>
       <c r="L61" s="16"/>
       <c r="M61" s="16"/>
       <c r="N61" s="16"/>
@@ -4742,31 +5168,31 @@
       <c r="V61" s="16"/>
     </row>
     <row r="62" spans="1:22" ht="39" thickBot="1">
-      <c r="A62" s="70" t="s">
+      <c r="A62" s="51" t="s">
         <v>311</v>
       </c>
-      <c r="B62" s="20"/>
-      <c r="C62" s="30" t="s">
+      <c r="B62" s="86"/>
+      <c r="C62" s="20" t="s">
         <v>312</v>
       </c>
-      <c r="D62" s="31" t="s">
+      <c r="D62" s="21" t="s">
         <v>313</v>
       </c>
-      <c r="E62" s="31" t="s">
+      <c r="E62" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="F62" s="31" t="s">
+      <c r="F62" s="21" t="s">
         <v>314</v>
       </c>
-      <c r="G62" s="41" t="s">
+      <c r="G62" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="H62" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="I62" s="71"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="30"/>
+      <c r="H62" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="I62" s="52"/>
+      <c r="J62" s="24"/>
+      <c r="K62" s="20"/>
       <c r="L62" s="16"/>
       <c r="M62" s="16"/>
       <c r="N62" s="16"/>
@@ -4780,31 +5206,31 @@
       <c r="V62" s="16"/>
     </row>
     <row r="63" spans="1:22" ht="39" thickBot="1">
-      <c r="A63" s="70" t="s">
+      <c r="A63" s="51" t="s">
         <v>315</v>
       </c>
-      <c r="B63" s="20"/>
-      <c r="C63" s="30" t="s">
+      <c r="B63" s="86"/>
+      <c r="C63" s="20" t="s">
         <v>316</v>
       </c>
-      <c r="D63" s="31" t="s">
+      <c r="D63" s="21" t="s">
         <v>317</v>
       </c>
-      <c r="E63" s="30" t="s">
+      <c r="E63" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="F63" s="31" t="s">
+      <c r="F63" s="21" t="s">
         <v>318</v>
       </c>
-      <c r="G63" s="41" t="s">
+      <c r="G63" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="H63" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="I63" s="71"/>
-      <c r="J63" s="37"/>
-      <c r="K63" s="30"/>
+      <c r="H63" s="73" t="s">
+        <v>397</v>
+      </c>
+      <c r="I63" s="52"/>
+      <c r="J63" s="24"/>
+      <c r="K63" s="20"/>
       <c r="L63" s="16"/>
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
@@ -4818,29 +5244,29 @@
       <c r="V63" s="16"/>
     </row>
     <row r="64" spans="1:22" ht="39" thickBot="1">
-      <c r="A64" s="72" t="s">
+      <c r="A64" s="53" t="s">
         <v>319</v>
       </c>
-      <c r="B64" s="73"/>
-      <c r="C64" s="74" t="s">
+      <c r="B64" s="89"/>
+      <c r="C64" s="54" t="s">
         <v>299</v>
       </c>
-      <c r="D64" s="75" t="s">
+      <c r="D64" s="55" t="s">
         <v>300</v>
       </c>
-      <c r="E64" s="74"/>
-      <c r="F64" s="75" t="s">
+      <c r="E64" s="54"/>
+      <c r="F64" s="55" t="s">
         <v>320</v>
       </c>
-      <c r="G64" s="78" t="s">
+      <c r="G64" s="57" t="s">
         <v>286</v>
       </c>
-      <c r="H64" s="76" t="s">
-        <v>217</v>
-      </c>
-      <c r="I64" s="77"/>
-      <c r="J64" s="37"/>
-      <c r="K64" s="30"/>
+      <c r="H64" s="74" t="s">
+        <v>397</v>
+      </c>
+      <c r="I64" s="56"/>
+      <c r="J64" s="24"/>
+      <c r="K64" s="20"/>
       <c r="L64" s="16"/>
       <c r="M64" s="16"/>
       <c r="N64" s="16"/>
@@ -4854,15 +5280,15 @@
       <c r="V64" s="16"/>
     </row>
     <row r="65" spans="1:22" ht="13.5" thickBot="1">
-      <c r="A65" s="38"/>
-      <c r="B65" s="38"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="38"/>
-      <c r="F65" s="38"/>
-      <c r="G65" s="38"/>
-      <c r="H65" s="38"/>
-      <c r="I65" s="38"/>
+      <c r="A65" s="25"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="25"/>
+      <c r="H65" s="25"/>
+      <c r="I65" s="25"/>
       <c r="J65" s="16"/>
       <c r="K65" s="16"/>
       <c r="L65" s="16"/>
@@ -5766,7 +6192,7 @@
       <c r="V102" s="16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I53" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I64" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="18">
     <mergeCell ref="A30:I30"/>
     <mergeCell ref="A54:I54"/>
@@ -5793,11 +6219,537 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EB391B-857A-416C-84A8-979130FEB219}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" style="58" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" style="58" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="58" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="58" customWidth="1"/>
+    <col min="5" max="5" width="44" style="58" customWidth="1"/>
+    <col min="6" max="7" width="31.5703125" style="58" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="58" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="58"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A1" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="37"/>
+    </row>
+    <row r="2" spans="1:9" ht="140.25">
+      <c r="A2" s="60" t="s">
+        <v>322</v>
+      </c>
+      <c r="B2" s="93" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2" s="68" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2" s="68" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2" s="68" t="s">
+        <v>326</v>
+      </c>
+      <c r="F2" s="68" t="s">
+        <v>327</v>
+      </c>
+      <c r="G2" s="68" t="s">
+        <v>285</v>
+      </c>
+      <c r="H2" s="71" t="s">
+        <v>397</v>
+      </c>
+      <c r="I2" s="61"/>
+    </row>
+    <row r="3" spans="1:9" ht="140.25">
+      <c r="A3" s="62" t="s">
+        <v>328</v>
+      </c>
+      <c r="B3" s="94"/>
+      <c r="C3" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I3" s="63"/>
+    </row>
+    <row r="4" spans="1:9" ht="140.25">
+      <c r="A4" s="62" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4" s="94" t="s">
+        <v>333</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I4" s="63"/>
+    </row>
+    <row r="5" spans="1:9" ht="63.75">
+      <c r="A5" s="62" t="s">
+        <v>336</v>
+      </c>
+      <c r="B5" s="94"/>
+      <c r="C5" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H5" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I5" s="63"/>
+    </row>
+    <row r="6" spans="1:9" ht="51">
+      <c r="A6" s="62" t="s">
+        <v>340</v>
+      </c>
+      <c r="B6" s="94"/>
+      <c r="C6" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H6" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I6" s="63"/>
+    </row>
+    <row r="7" spans="1:9" ht="51">
+      <c r="A7" s="62" t="s">
+        <v>345</v>
+      </c>
+      <c r="B7" s="94" t="s">
+        <v>346</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I7" s="63"/>
+    </row>
+    <row r="8" spans="1:9" ht="51">
+      <c r="A8" s="62" t="s">
+        <v>350</v>
+      </c>
+      <c r="B8" s="94"/>
+      <c r="C8" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H8" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I8" s="63"/>
+    </row>
+    <row r="9" spans="1:9" ht="51">
+      <c r="A9" s="62" t="s">
+        <v>353</v>
+      </c>
+      <c r="B9" s="94"/>
+      <c r="C9" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H9" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I9" s="63"/>
+    </row>
+    <row r="10" spans="1:9" ht="51">
+      <c r="A10" s="62" t="s">
+        <v>358</v>
+      </c>
+      <c r="B10" s="94" t="s">
+        <v>359</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H10" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I10" s="63"/>
+    </row>
+    <row r="11" spans="1:9" ht="51">
+      <c r="A11" s="62" t="s">
+        <v>364</v>
+      </c>
+      <c r="B11" s="94"/>
+      <c r="C11" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H11" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I11" s="63"/>
+    </row>
+    <row r="12" spans="1:9" ht="51">
+      <c r="A12" s="62" t="s">
+        <v>366</v>
+      </c>
+      <c r="B12" s="94" t="s">
+        <v>367</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H12" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I12" s="63"/>
+    </row>
+    <row r="13" spans="1:9" ht="51">
+      <c r="A13" s="62" t="s">
+        <v>371</v>
+      </c>
+      <c r="B13" s="94"/>
+      <c r="C13" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H13" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I13" s="63"/>
+    </row>
+    <row r="14" spans="1:9" ht="51">
+      <c r="A14" s="62" t="s">
+        <v>374</v>
+      </c>
+      <c r="B14" s="94"/>
+      <c r="C14" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H14" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I14" s="63"/>
+    </row>
+    <row r="15" spans="1:9" ht="51">
+      <c r="A15" s="62" t="s">
+        <v>376</v>
+      </c>
+      <c r="B15" s="94"/>
+      <c r="C15" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H15" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I15" s="63"/>
+    </row>
+    <row r="16" spans="1:9" ht="51">
+      <c r="A16" s="62" t="s">
+        <v>381</v>
+      </c>
+      <c r="B16" s="94" t="s">
+        <v>382</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H16" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I16" s="63"/>
+    </row>
+    <row r="17" spans="1:9" ht="51">
+      <c r="A17" s="62" t="s">
+        <v>386</v>
+      </c>
+      <c r="B17" s="94"/>
+      <c r="C17" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H17" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I17" s="63"/>
+    </row>
+    <row r="18" spans="1:9" ht="51">
+      <c r="A18" s="62" t="s">
+        <v>389</v>
+      </c>
+      <c r="B18" s="66" t="s">
+        <v>390</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="H18" s="59" t="s">
+        <v>397</v>
+      </c>
+      <c r="I18" s="63"/>
+    </row>
+    <row r="19" spans="1:9" ht="51.75" thickBot="1">
+      <c r="A19" s="64" t="s">
+        <v>393</v>
+      </c>
+      <c r="B19" s="67" t="s">
+        <v>394</v>
+      </c>
+      <c r="C19" s="69" t="s">
+        <v>395</v>
+      </c>
+      <c r="D19" s="69" t="s">
+        <v>325</v>
+      </c>
+      <c r="E19" s="69" t="s">
+        <v>356</v>
+      </c>
+      <c r="F19" s="69" t="s">
+        <v>396</v>
+      </c>
+      <c r="G19" s="69" t="s">
+        <v>286</v>
+      </c>
+      <c r="H19" s="72" t="s">
+        <v>397</v>
+      </c>
+      <c r="I19" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A068CEBD-4C22-427A-8D4A-7C4C89933131}">
   <dimension ref="B2:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5825,7 +6777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5870,12 +6822,12 @@
     </row>
     <row r="2" spans="1:20" ht="12.75" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -8058,7 +9010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -8242,7 +9194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -8336,7 +9288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -8576,7 +9528,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>